<commit_message>
working on transition matrix
</commit_message>
<xml_diff>
--- a/data/ghg data.xlsx
+++ b/data/ghg data.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://hecmtl-my.sharepoint.com/personal/thien-duy_tran_hec_ca/Documents/esg/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TTD\OneDrive - HEC Montréal\esg\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="10" documentId="8_{C8D9E0C4-7903-4131-B376-9C2B77E53766}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{B38BA6EB-6401-4233-99B6-E4956122EDC9}"/>
+  <xr:revisionPtr revIDLastSave="177" documentId="8_{C8D9E0C4-7903-4131-B376-9C2B77E53766}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{4D9835C6-3AF5-426D-850C-CD66B539C685}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{276B7657-227E-447A-B24C-1F2259F8264B}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Observations" sheetId="1" r:id="rId1"/>
+    <sheet name="Transition Matrix" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="29">
   <si>
     <t>All</t>
   </si>
@@ -45,13 +46,91 @@
   </si>
   <si>
     <t>Daily</t>
+  </si>
+  <si>
+    <t>Monthly Data</t>
+  </si>
+  <si>
+    <t>Daily Data</t>
+  </si>
+  <si>
+    <t>2009-2017</t>
+  </si>
+  <si>
+    <t>1995-2018</t>
+  </si>
+  <si>
+    <t>SPMIM</t>
+  </si>
+  <si>
+    <t>Ratio</t>
+  </si>
+  <si>
+    <t>N obs</t>
+  </si>
+  <si>
+    <t>N firms</t>
+  </si>
+  <si>
+    <t>N obs - scope 1 &amp; 2</t>
+  </si>
+  <si>
+    <t>N obs - scope 3</t>
+  </si>
+  <si>
+    <t>N obs - scope 1 &amp; 2 (%)</t>
+  </si>
+  <si>
+    <t>N obs - scope 3 (%)</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Total obs</t>
+  </si>
+  <si>
+    <t>Obs with scope 3</t>
+  </si>
+  <si>
+    <t>Scope 1 &amp; 2 (%)</t>
+  </si>
+  <si>
+    <t>Scope 3 (%)</t>
+  </si>
+  <si>
+    <t>Obs with scope 1 &amp; 2</t>
+  </si>
+  <si>
+    <t>Total firms</t>
+  </si>
+  <si>
+    <t>Firms with scope 1 &amp; 2</t>
+  </si>
+  <si>
+    <t>Firms with scope 3</t>
+  </si>
+  <si>
+    <t>Green</t>
+  </si>
+  <si>
+    <t>Neutral</t>
+  </si>
+  <si>
+    <t>Brown</t>
+  </si>
+  <si>
+    <t>Non-Disclosed</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0%"/>
+  </numFmts>
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -80,16 +159,43 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -97,12 +203,30 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -114,10 +238,30 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="4" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="1" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="5">
+    <cellStyle name="20% - Accent5" xfId="4" builtinId="46"/>
+    <cellStyle name="40% - Accent1" xfId="3" builtinId="31"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="2" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -130,6 +274,61 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>1200150</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="3" name="Straight Connector 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9C9051FC-930A-47A9-A778-17E116BE053E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8515350" y="2066925"/>
+          <a:ext cx="3924300" cy="1476375"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -429,15 +628,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1FAC0BC2-575D-4EBB-AA69-02907ED29842}">
-  <dimension ref="A1:I16"/>
+  <dimension ref="A1:W30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P11" sqref="P11"/>
+      <selection activeCell="Y7" sqref="Y7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="13" max="13" width="22.5703125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:23">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -462,11 +664,31 @@
       <c r="I1">
         <v>2018</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" ht="18">
-      <c r="A2" s="1"/>
-    </row>
-    <row r="3" spans="1:9">
+      <c r="M1" s="6"/>
+      <c r="N1" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="O1" s="9"/>
+      <c r="P1" s="9"/>
+      <c r="Q1" s="9"/>
+      <c r="R1" s="9"/>
+      <c r="S1" s="9"/>
+    </row>
+    <row r="2" spans="1:23">
+      <c r="M2" s="6"/>
+      <c r="N2" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="O2" s="7"/>
+      <c r="P2" s="7"/>
+      <c r="Q2" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="R2" s="7"/>
+      <c r="S2" s="7"/>
+    </row>
+    <row r="3" spans="1:23" ht="18">
+      <c r="A3" s="1"/>
       <c r="B3">
         <v>1458310</v>
       </c>
@@ -485,17 +707,35 @@
       <c r="I3">
         <v>0.26983774654368198</v>
       </c>
-    </row>
-    <row r="4" spans="1:9">
-      <c r="A4" s="2"/>
+      <c r="M3" s="6"/>
+      <c r="N3" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="O3" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="P3" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q3" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="R3" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="S3" s="8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23">
       <c r="B4">
-        <v>14276</v>
+        <v>54660</v>
       </c>
       <c r="C4">
-        <v>3351</v>
+        <v>46642</v>
       </c>
       <c r="D4">
-        <v>0.234729616138975</v>
+        <v>0.85331137943651703</v>
       </c>
       <c r="G4">
         <v>14276</v>
@@ -506,17 +746,60 @@
       <c r="I4">
         <v>0.234729616138975</v>
       </c>
-    </row>
-    <row r="5" spans="1:9">
-      <c r="A5" s="3"/>
+      <c r="M4" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="N4" s="8">
+        <f>B3</f>
+        <v>1458310</v>
+      </c>
+      <c r="O4" s="8">
+        <f>C3</f>
+        <v>393576</v>
+      </c>
+      <c r="P4" s="10">
+        <f>O4/N4</f>
+        <v>0.26988500387434772</v>
+      </c>
+      <c r="Q4" s="8">
+        <f>B12</f>
+        <v>404614</v>
+      </c>
+      <c r="R4" s="8">
+        <f t="shared" ref="R4:R6" si="0">C12</f>
+        <v>144810</v>
+      </c>
+      <c r="S4" s="10">
+        <f>R4/Q4</f>
+        <v>0.35789666200378634</v>
+      </c>
+      <c r="T4">
+        <f>Q4-N4</f>
+        <v>-1053696</v>
+      </c>
+      <c r="U4">
+        <f>R4-O4</f>
+        <v>-248766</v>
+      </c>
+      <c r="V4" s="5">
+        <f>T4/N4</f>
+        <v>-0.72254596073537181</v>
+      </c>
+      <c r="W4" s="5">
+        <f>U4/O4</f>
+        <v>-0.63206597963290445</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23">
+      <c r="A5" s="2"/>
       <c r="B5">
-        <v>54660</v>
+        <v>25332</v>
       </c>
       <c r="C5">
-        <v>46642</v>
+        <v>21870</v>
       </c>
       <c r="D5">
-        <v>0.85331137943651703</v>
+        <v>0.86333491236380899</v>
       </c>
       <c r="G5">
         <v>1146302</v>
@@ -527,17 +810,60 @@
       <c r="I5">
         <v>0.85329433255808695</v>
       </c>
-    </row>
-    <row r="6" spans="1:9">
-      <c r="A6" s="4"/>
+      <c r="M5" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="N5" s="8">
+        <f>B4</f>
+        <v>54660</v>
+      </c>
+      <c r="O5" s="8">
+        <f>C4</f>
+        <v>46642</v>
+      </c>
+      <c r="P5" s="10">
+        <f>O5/N5</f>
+        <v>0.85331137943651669</v>
+      </c>
+      <c r="Q5" s="8">
+        <f t="shared" ref="Q5:Q6" si="1">B13</f>
+        <v>40430</v>
+      </c>
+      <c r="R5" s="8">
+        <f t="shared" si="0"/>
+        <v>35562</v>
+      </c>
+      <c r="S5" s="10">
+        <f>R5/Q5</f>
+        <v>0.87959436062329954</v>
+      </c>
+      <c r="T5">
+        <f>Q5-N5</f>
+        <v>-14230</v>
+      </c>
+      <c r="U5">
+        <f>R5-O5</f>
+        <v>-11080</v>
+      </c>
+      <c r="V5" s="5">
+        <f>T5/N5</f>
+        <v>-0.26033662641785582</v>
+      </c>
+      <c r="W5" s="5">
+        <f>U5/O5</f>
+        <v>-0.23755413575747181</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23">
+      <c r="A6" s="3"/>
       <c r="B6">
-        <v>25332</v>
+        <v>14276</v>
       </c>
       <c r="C6">
-        <v>21870</v>
+        <v>3351</v>
       </c>
       <c r="D6">
-        <v>0.86333491236380899</v>
+        <v>0.234729616138975</v>
       </c>
       <c r="G6">
         <v>531163</v>
@@ -548,116 +874,314 @@
       <c r="I6">
         <v>0.86329620097785398</v>
       </c>
-    </row>
-    <row r="7" spans="1:9">
-      <c r="A7" s="3"/>
+      <c r="M6" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="N6" s="8">
+        <f>B5</f>
+        <v>25332</v>
+      </c>
+      <c r="O6" s="8">
+        <f>C5</f>
+        <v>21870</v>
+      </c>
+      <c r="P6" s="10">
+        <f>O6/N6</f>
+        <v>0.86333491236380866</v>
+      </c>
+      <c r="Q6" s="8">
+        <f t="shared" si="1"/>
+        <v>21353</v>
+      </c>
+      <c r="R6" s="8">
+        <f t="shared" si="0"/>
+        <v>19229</v>
+      </c>
+      <c r="S6" s="10">
+        <f>R6/Q6</f>
+        <v>0.90052919964407807</v>
+      </c>
+      <c r="T6">
+        <f>Q6-N6</f>
+        <v>-3979</v>
+      </c>
+      <c r="U6">
+        <f>R6-O6</f>
+        <v>-2641</v>
+      </c>
+      <c r="V6" s="5">
+        <f>T6/N6</f>
+        <v>-0.15707405652929102</v>
+      </c>
+      <c r="W6" s="5">
+        <f>U6/O6</f>
+        <v>-0.12075903063557385</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23">
+      <c r="A7" s="4"/>
       <c r="B7">
-        <v>54972</v>
+        <v>648</v>
       </c>
       <c r="C7">
-        <v>46930</v>
+        <v>543</v>
       </c>
       <c r="D7">
-        <v>0.85370734191952302</v>
-      </c>
-      <c r="G7">
-        <v>1152844</v>
-      </c>
-      <c r="H7">
-        <v>984173</v>
-      </c>
-      <c r="I7">
-        <v>0.85369139276432904</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9">
-      <c r="A8" s="4"/>
+        <v>0.83796296296296302</v>
+      </c>
+      <c r="M7" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="N7" s="10">
+        <f>N5/N$4</f>
+        <v>3.7481742565023894E-2</v>
+      </c>
+      <c r="O7" s="10">
+        <f>O5/O$4</f>
+        <v>0.11850824237250239</v>
+      </c>
+      <c r="P7" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q7" s="10">
+        <f>Q5/Q$4</f>
+        <v>9.9922395171694503E-2</v>
+      </c>
+      <c r="R7" s="10">
+        <f>R5/R$4</f>
+        <v>0.24557696291692563</v>
+      </c>
+      <c r="S7" s="10" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23">
+      <c r="A8" s="3"/>
       <c r="B8">
-        <v>25020</v>
+        <v>382</v>
       </c>
       <c r="C8">
-        <v>21582</v>
+        <v>333</v>
       </c>
       <c r="D8">
-        <v>0.86258992805755397</v>
-      </c>
-      <c r="G8">
-        <v>524621</v>
-      </c>
-      <c r="H8">
-        <v>452511</v>
-      </c>
-      <c r="I8">
-        <v>0.86254839207732803</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9">
-      <c r="A10" t="s">
+        <v>0.87172774869109904</v>
+      </c>
+      <c r="M8" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="N8" s="10">
+        <f>N6/N$4</f>
+        <v>1.7370792218389781E-2</v>
+      </c>
+      <c r="O8" s="10">
+        <f>O6/O$4</f>
+        <v>5.5567412647112631E-2</v>
+      </c>
+      <c r="P8" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q8" s="10">
+        <f>Q6/Q$4</f>
+        <v>5.2773754739084661E-2</v>
+      </c>
+      <c r="R8" s="10">
+        <f>R6/R$4</f>
+        <v>0.13278779089841861</v>
+      </c>
+      <c r="S8" s="10" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:23">
+      <c r="A9" s="4"/>
+      <c r="B9">
+        <v>372</v>
+      </c>
+      <c r="C9">
+        <v>324</v>
+      </c>
+      <c r="D9">
+        <v>0.87096774193548399</v>
+      </c>
+      <c r="M9" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="N9" s="8">
+        <f>B6</f>
+        <v>14276</v>
+      </c>
+      <c r="O9" s="8">
+        <f>C6</f>
+        <v>3351</v>
+      </c>
+      <c r="P9" s="10">
+        <f>O9/N9</f>
+        <v>0.2347296161389745</v>
+      </c>
+      <c r="Q9" s="8">
+        <f>B15</f>
+        <v>5985</v>
+      </c>
+      <c r="R9" s="8">
+        <f>C15</f>
+        <v>1887</v>
+      </c>
+      <c r="S9" s="10">
+        <f>R9/Q9</f>
+        <v>0.31528822055137845</v>
+      </c>
+      <c r="T9">
+        <f>Q9-N9</f>
+        <v>-8291</v>
+      </c>
+      <c r="U9">
+        <f>R9-O9</f>
+        <v>-1464</v>
+      </c>
+      <c r="V9" s="5">
+        <f>T9/N9</f>
+        <v>-0.58076492014569903</v>
+      </c>
+      <c r="W9" s="5">
+        <f>U9/O9</f>
+        <v>-0.43688451208594448</v>
+      </c>
+    </row>
+    <row r="10" spans="1:23">
+      <c r="M10" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="N10" s="8">
+        <f>B7</f>
+        <v>648</v>
+      </c>
+      <c r="O10" s="8">
+        <f>C7</f>
+        <v>543</v>
+      </c>
+      <c r="P10" s="10">
+        <f t="shared" ref="P10:P11" si="2">O10/N10</f>
+        <v>0.83796296296296291</v>
+      </c>
+      <c r="Q10" s="8">
+        <f t="shared" ref="Q10:R10" si="3">B16</f>
+        <v>615</v>
+      </c>
+      <c r="R10" s="8">
+        <f t="shared" si="3"/>
+        <v>511</v>
+      </c>
+      <c r="S10" s="10">
+        <f t="shared" ref="S10:S11" si="4">R10/Q10</f>
+        <v>0.83089430894308947</v>
+      </c>
+      <c r="T10">
+        <f>Q10-N10</f>
+        <v>-33</v>
+      </c>
+      <c r="U10">
+        <f>R10-O10</f>
+        <v>-32</v>
+      </c>
+      <c r="V10" s="5">
+        <f>T10/N10</f>
+        <v>-5.0925925925925923E-2</v>
+      </c>
+      <c r="W10" s="5">
+        <f>U10/O10</f>
+        <v>-5.8931860036832415E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:23">
+      <c r="A11" t="s">
         <v>2</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B11" t="s">
         <v>1</v>
       </c>
-      <c r="C10">
+      <c r="C11">
         <v>2009</v>
       </c>
-      <c r="D10">
+      <c r="D11">
         <v>2017</v>
       </c>
-      <c r="F10" t="s">
+      <c r="F11" t="s">
         <v>3</v>
       </c>
-      <c r="G10" t="s">
+      <c r="G11" t="s">
         <v>1</v>
       </c>
-      <c r="H10">
+      <c r="H11">
         <v>2009</v>
       </c>
-      <c r="I10">
+      <c r="I11">
         <v>2017</v>
       </c>
-    </row>
-    <row r="11" spans="1:9">
-      <c r="B11">
+      <c r="M11" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="N11" s="8">
+        <f>B8</f>
+        <v>382</v>
+      </c>
+      <c r="O11" s="8">
+        <f>C8</f>
+        <v>333</v>
+      </c>
+      <c r="P11" s="10">
+        <f t="shared" si="2"/>
+        <v>0.87172774869109948</v>
+      </c>
+      <c r="Q11" s="8">
+        <f t="shared" ref="Q11:R11" si="5">B17</f>
+        <v>362</v>
+      </c>
+      <c r="R11" s="8">
+        <f t="shared" si="5"/>
+        <v>313</v>
+      </c>
+      <c r="S11" s="10">
+        <f t="shared" si="4"/>
+        <v>0.86464088397790051</v>
+      </c>
+      <c r="T11">
+        <f>Q11-N11</f>
+        <v>-20</v>
+      </c>
+      <c r="U11">
+        <f>R11-O11</f>
+        <v>-20</v>
+      </c>
+      <c r="V11" s="5">
+        <f>T11/N11</f>
+        <v>-5.2356020942408377E-2</v>
+      </c>
+      <c r="W11" s="5">
+        <f>U11/O11</f>
+        <v>-6.006006006006006E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:23">
+      <c r="B12">
         <v>404614</v>
       </c>
-      <c r="C11">
+      <c r="C12">
         <v>144810</v>
       </c>
-      <c r="D11">
-        <v>0.35789670000000001</v>
-      </c>
-      <c r="G11">
+      <c r="D12">
+        <v>0.357896662003786</v>
+      </c>
+      <c r="G12">
         <v>8485090</v>
       </c>
-      <c r="H11">
+      <c r="H12">
         <v>3036958</v>
       </c>
-      <c r="I11">
+      <c r="I12">
         <v>0.35791700500524998</v>
       </c>
     </row>
-    <row r="12" spans="1:9">
-      <c r="B12">
-        <v>5985</v>
-      </c>
-      <c r="C12">
-        <v>1887</v>
-      </c>
-      <c r="D12">
-        <v>0.31528820000000002</v>
-      </c>
-      <c r="G12">
-        <v>5985</v>
-      </c>
-      <c r="H12">
-        <v>1887</v>
-      </c>
-      <c r="I12">
-        <v>0.31528822055137801</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9">
+    <row r="13" spans="1:23">
       <c r="B13">
         <v>40430</v>
       </c>
@@ -665,19 +1189,19 @@
         <v>35562</v>
       </c>
       <c r="D13">
-        <v>0.8795944</v>
+        <v>0.87959436062329999</v>
       </c>
       <c r="G13">
-        <v>847907</v>
+        <v>5985</v>
       </c>
       <c r="H13">
-        <v>745810</v>
+        <v>1887</v>
       </c>
       <c r="I13">
-        <v>0.87958938893062599</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9">
+        <v>0.31528822055137801</v>
+      </c>
+    </row>
+    <row r="14" spans="1:23">
       <c r="B14">
         <v>21353</v>
       </c>
@@ -685,80 +1209,356 @@
         <v>19229</v>
       </c>
       <c r="D14">
-        <v>0.90052920000000003</v>
+        <v>0.90052919964407796</v>
       </c>
       <c r="G14">
+        <v>847907</v>
+      </c>
+      <c r="H14">
+        <v>745810</v>
+      </c>
+      <c r="I14">
+        <v>0.87958938893062599</v>
+      </c>
+    </row>
+    <row r="15" spans="1:23">
+      <c r="B15">
+        <v>5985</v>
+      </c>
+      <c r="C15">
+        <v>1887</v>
+      </c>
+      <c r="D15">
+        <v>0.31528822055137801</v>
+      </c>
+      <c r="G15">
         <v>447775</v>
       </c>
-      <c r="H14">
+      <c r="H15">
         <v>403225</v>
       </c>
-      <c r="I14">
+      <c r="I15">
         <v>0.90050806766791403</v>
       </c>
     </row>
-    <row r="15" spans="1:9">
-      <c r="B15">
-        <v>40550</v>
-      </c>
-      <c r="C15">
-        <v>35682</v>
-      </c>
-      <c r="D15">
-        <v>0.87995069999999997</v>
-      </c>
-      <c r="G15">
-        <v>850427</v>
-      </c>
-      <c r="H15">
-        <v>748330</v>
-      </c>
-      <c r="I15">
-        <v>0.87994619173662203</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9">
+    <row r="16" spans="1:23">
       <c r="B16">
-        <v>21233</v>
+        <v>615</v>
       </c>
       <c r="C16">
-        <v>19109</v>
+        <v>511</v>
       </c>
       <c r="D16">
-        <v>0.89996699999999996</v>
-      </c>
-      <c r="G16">
-        <v>445255</v>
-      </c>
-      <c r="H16">
-        <v>400705</v>
-      </c>
-      <c r="I16">
-        <v>0.89994497535120299</v>
-      </c>
+        <v>0.83089430894308902</v>
+      </c>
+    </row>
+    <row r="17" spans="2:19">
+      <c r="B17">
+        <v>362</v>
+      </c>
+      <c r="C17">
+        <v>313</v>
+      </c>
+      <c r="D17">
+        <v>0.86464088397790095</v>
+      </c>
+    </row>
+    <row r="18" spans="2:19">
+      <c r="B18">
+        <v>361</v>
+      </c>
+      <c r="C18">
+        <v>312</v>
+      </c>
+      <c r="D18">
+        <v>0.86426592797783897</v>
+      </c>
+    </row>
+    <row r="22" spans="2:19">
+      <c r="M22" s="6"/>
+      <c r="N22" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="O22" s="9"/>
+      <c r="P22" s="9"/>
+      <c r="Q22" s="9"/>
+      <c r="R22" s="9"/>
+      <c r="S22" s="9"/>
+    </row>
+    <row r="23" spans="2:19">
+      <c r="M23" s="6"/>
+      <c r="N23" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="O23" s="7"/>
+      <c r="P23" s="7"/>
+      <c r="Q23" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="R23" s="7"/>
+      <c r="S23" s="7"/>
+    </row>
+    <row r="24" spans="2:19">
+      <c r="M24" s="6"/>
+      <c r="N24" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="O24" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="P24" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q24" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="R24" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="S24" s="8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="25" spans="2:19">
+      <c r="M25" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="N25" s="8">
+        <v>30599040</v>
+      </c>
+      <c r="O25" s="8">
+        <v>8256776</v>
+      </c>
+      <c r="P25" s="10">
+        <f>O25/N25</f>
+        <v>0.26983774654368242</v>
+      </c>
+      <c r="Q25" s="8">
+        <v>8485090</v>
+      </c>
+      <c r="R25" s="8">
+        <v>3036958</v>
+      </c>
+      <c r="S25" s="10">
+        <f>R25/Q25</f>
+        <v>0.35791700500525037</v>
+      </c>
+    </row>
+    <row r="26" spans="2:19">
+      <c r="M26" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="N26" s="8">
+        <v>14276</v>
+      </c>
+      <c r="O26" s="8">
+        <v>3351</v>
+      </c>
+      <c r="P26" s="10">
+        <f t="shared" ref="P26:P28" si="6">O26/N26</f>
+        <v>0.2347296161389745</v>
+      </c>
+      <c r="Q26" s="8">
+        <v>5985</v>
+      </c>
+      <c r="R26" s="8">
+        <v>1887</v>
+      </c>
+      <c r="S26" s="10">
+        <f t="shared" ref="S26:S28" si="7">R26/Q26</f>
+        <v>0.31528822055137845</v>
+      </c>
+    </row>
+    <row r="27" spans="2:19">
+      <c r="M27" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="N27" s="8">
+        <v>1146302</v>
+      </c>
+      <c r="O27" s="8">
+        <v>978133</v>
+      </c>
+      <c r="P27" s="10">
+        <f t="shared" si="6"/>
+        <v>0.85329433255808673</v>
+      </c>
+      <c r="Q27" s="8">
+        <v>847907</v>
+      </c>
+      <c r="R27" s="8">
+        <v>745810</v>
+      </c>
+      <c r="S27" s="10">
+        <f t="shared" si="7"/>
+        <v>0.87958938893062566</v>
+      </c>
+    </row>
+    <row r="28" spans="2:19">
+      <c r="M28" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="N28" s="8">
+        <v>531163</v>
+      </c>
+      <c r="O28" s="8">
+        <v>458551</v>
+      </c>
+      <c r="P28" s="10">
+        <f t="shared" si="6"/>
+        <v>0.86329620097785431</v>
+      </c>
+      <c r="Q28" s="8">
+        <v>447775</v>
+      </c>
+      <c r="R28" s="8">
+        <v>403225</v>
+      </c>
+      <c r="S28" s="10">
+        <f t="shared" si="7"/>
+        <v>0.90050806766791358</v>
+      </c>
+    </row>
+    <row r="29" spans="2:19">
+      <c r="M29" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="N29" s="10">
+        <f>N27/N$25</f>
+        <v>3.7462024952416809E-2</v>
+      </c>
+      <c r="O29" s="10">
+        <f>O27/O$25</f>
+        <v>0.11846427709798595</v>
+      </c>
+      <c r="P29" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q29" s="10">
+        <f>Q27/Q$25</f>
+        <v>9.9929052019483586E-2</v>
+      </c>
+      <c r="R29" s="10">
+        <f>R27/R$25</f>
+        <v>0.24557797638294634</v>
+      </c>
+      <c r="S29" s="10" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="30" spans="2:19">
+      <c r="M30" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="N30" s="10">
+        <f>N28/N$25</f>
+        <v>1.7358812564054298E-2</v>
+      </c>
+      <c r="O30" s="10">
+        <f>O28/O$25</f>
+        <v>5.553632555854731E-2</v>
+      </c>
+      <c r="P30" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q30" s="10">
+        <f>Q28/Q$25</f>
+        <v>5.2771980026139968E-2</v>
+      </c>
+      <c r="R30" s="10">
+        <f>R28/R$25</f>
+        <v>0.13277266264465956</v>
+      </c>
+      <c r="S30" s="10" t="s">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="N1:S1"/>
+    <mergeCell ref="Q2:S2"/>
+    <mergeCell ref="N2:P2"/>
+    <mergeCell ref="N22:S22"/>
+    <mergeCell ref="N23:P23"/>
+    <mergeCell ref="Q23:S23"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{841F1098-67C7-41B6-ADDB-E324A597535D}">
+  <dimension ref="A2:E6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J10" sqref="J10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
+    <col min="2" max="5" width="13.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:5" ht="27" customHeight="1">
+      <c r="A2" s="11"/>
+      <c r="B2" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="E2" s="11" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="27" customHeight="1">
+      <c r="A3" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" s="11"/>
+      <c r="C3" s="11"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="11"/>
+    </row>
+    <row r="4" spans="1:5" ht="27" customHeight="1">
+      <c r="A4" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4" s="11"/>
+      <c r="C4" s="11"/>
+      <c r="D4" s="11"/>
+      <c r="E4" s="11"/>
+    </row>
+    <row r="5" spans="1:5" ht="27" customHeight="1">
+      <c r="A5" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5" s="11"/>
+      <c r="C5" s="11"/>
+      <c r="D5" s="11"/>
+      <c r="E5" s="11"/>
+    </row>
+    <row r="6" spans="1:5" ht="27" customHeight="1">
+      <c r="A6" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="B6" s="11"/>
+      <c r="C6" s="11"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100DC7FD9415D2401459AC7BCE314D31F5A" ma:contentTypeVersion="10" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="8c8b8c1a242a721cfd851b431e709e1f">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="179859d2-a65d-4f70-b758-5dd1739daa4e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="9368ac5f987cc59676eee1cde973b1fb" ns3:_="">
     <xsd:import namespace="179859d2-a65d-4f70-b758-5dd1739daa4e"/>
@@ -942,24 +1742,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{26B2706D-9832-41EF-BF90-2EC1DE47AF21}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C9D1B1C1-A102-4FEC-90A6-DF5EB0B7B3A9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{443C75FB-D95B-4839-94B9-2D7FE6BCB1E9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -975,4 +1773,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C9D1B1C1-A102-4FEC-90A6-DF5EB0B7B3A9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{26B2706D-9832-41EF-BF90-2EC1DE47AF21}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>